<commit_message>
Updating food processing technology costs calculation spreadsheet
</commit_message>
<xml_diff>
--- a/food_processing_tech_costs_final.xlsx
+++ b/food_processing_tech_costs_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spei632\Documents\GCAM_industry\food_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E605BA2-012A-446A-8F25-9BEFA26846E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E284A101-F2C1-465F-ADE8-EC6BD98F1ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="-20360" windowWidth="22170" windowHeight="17450" xr2:uid="{34AE4EF8-B5B7-475C-B9E2-D77ABC490651}"/>
+    <workbookView xWindow="1970" yWindow="-16450" windowWidth="23980" windowHeight="14940" xr2:uid="{34AE4EF8-B5B7-475C-B9E2-D77ABC490651}"/>
   </bookViews>
   <sheets>
     <sheet name="process heat technologies" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Constants</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Sources: based on the range as a function of temperature for parabolic trough collectors from appendices of "Renewable Energy Options for Industrial Process Heat", https://arena.gov.au/assets/2019/11/appendices-renewable-energy-options-for-industrial-process-heat.pdf</t>
+  </si>
+  <si>
+    <t>capital ratio</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,6 +607,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0F238C-106E-4388-8591-908DEC2A4380}">
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,7 +944,7 @@
     <col min="10" max="10" width="12.453125" customWidth="1"/>
     <col min="11" max="11" width="13.7265625" customWidth="1"/>
     <col min="12" max="12" width="8.08984375" customWidth="1"/>
-    <col min="13" max="14" width="13" customWidth="1"/>
+    <col min="13" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1078,7 +1084,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
@@ -1094,8 +1100,9 @@
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="2:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B18" s="14" t="s">
         <v>11</v>
       </c>
@@ -1133,12 +1140,15 @@
       <c r="N18" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="O18" s="1"/>
-      <c r="P18" s="12" t="s">
+      <c r="O18" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:19" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
@@ -1185,11 +1195,15 @@
         <f>ROUND(M19,2)</f>
         <v>1.08</v>
       </c>
-      <c r="P19" s="30" t="s">
+      <c r="O19" s="21">
+        <f>F19/K19</f>
+        <v>0.61272960003223997</v>
+      </c>
+      <c r="Q19" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B20" s="16" t="s">
         <v>39</v>
       </c>
@@ -1236,11 +1250,15 @@
         <f t="shared" ref="N20:N22" si="4">ROUND(M20,2)</f>
         <v>2.75</v>
       </c>
-      <c r="P20" s="30" t="s">
+      <c r="O20" s="21">
+        <f>F20/K20</f>
+        <v>0.92407318806540972</v>
+      </c>
+      <c r="Q20" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B21" s="16" t="s">
         <v>14</v>
       </c>
@@ -1287,11 +1305,15 @@
         <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
-      <c r="P21" s="30" t="s">
+      <c r="O21" s="21">
+        <f>F21/K21</f>
+        <v>0.70295570486016756</v>
+      </c>
+      <c r="Q21" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:19" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="17" t="s">
         <v>15</v>
       </c>
@@ -1338,12 +1360,18 @@
         <f t="shared" si="4"/>
         <v>2.67</v>
       </c>
-      <c r="P22" s="30" t="s">
+      <c r="O22" s="21">
+        <f>F22/K22</f>
+        <v>0.92166012891796267</v>
+      </c>
+      <c r="Q22" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O23" s="23"/>
+    </row>
+    <row r="24" spans="2:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>42</v>
       </c>
@@ -1365,8 +1393,9 @@
       <c r="N24" s="29" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="O24" s="52"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B25" s="19" t="s">
         <v>33</v>
       </c>
@@ -1392,14 +1421,15 @@
         <f t="shared" ref="N25:N28" si="5">ROUND(M25,2)</f>
         <v>1.08</v>
       </c>
-      <c r="O25" s="10"/>
-      <c r="P25" s="51" t="s">
+      <c r="O25" s="21"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S25" s="10"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B26" s="19" t="s">
         <v>34</v>
       </c>
@@ -1425,14 +1455,15 @@
         <f t="shared" si="5"/>
         <v>2.7</v>
       </c>
-      <c r="O26" s="10"/>
-      <c r="P26" s="50" t="s">
+      <c r="O26" s="21"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S26" s="10"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B27" s="19" t="s">
         <v>35</v>
       </c>
@@ -1458,14 +1489,15 @@
         <f t="shared" si="5"/>
         <v>2.7</v>
       </c>
-      <c r="O27" s="10"/>
-      <c r="P27" s="50" t="s">
+      <c r="O27" s="21"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S27" s="10"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B28" s="19" t="s">
         <v>44</v>
       </c>
@@ -1491,12 +1523,13 @@
         <f t="shared" si="5"/>
         <v>1.08</v>
       </c>
-      <c r="O28" s="10"/>
+      <c r="O28" s="21"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S28" s="10"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B29" s="19"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1510,12 +1543,13 @@
       <c r="L29" s="10"/>
       <c r="M29" s="32"/>
       <c r="N29" s="27"/>
-      <c r="O29" s="10"/>
+      <c r="O29" s="21"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S29" s="10"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B30" s="19" t="s">
         <v>29</v>
       </c>
@@ -1539,12 +1573,13 @@
         <f t="shared" ref="N30:N32" si="7">ROUND(M30,2)</f>
         <v>2.75</v>
       </c>
-      <c r="O30" s="10"/>
+      <c r="O30" s="21"/>
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S30" s="10"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B31" s="19" t="s">
         <v>30</v>
       </c>
@@ -1568,12 +1603,13 @@
         <f t="shared" si="7"/>
         <v>6.88</v>
       </c>
-      <c r="O31" s="10"/>
+      <c r="O31" s="21"/>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
-    </row>
-    <row r="32" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S31" s="10"/>
+    </row>
+    <row r="32" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="20" t="s">
         <v>36</v>
       </c>
@@ -1597,12 +1633,13 @@
         <f t="shared" si="7"/>
         <v>6.88</v>
       </c>
-      <c r="O32" s="10"/>
+      <c r="O32" s="21"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
-    </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S32" s="10"/>
+    </row>
+    <row r="33" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="18"/>
       <c r="B33" s="41"/>
       <c r="C33" s="18"/>
@@ -1617,14 +1654,17 @@
       <c r="L33" s="18"/>
       <c r="M33" s="42"/>
       <c r="N33" s="42"/>
-      <c r="O33" s="18"/>
+      <c r="O33" s="42"/>
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
-    </row>
-    <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T33" s="18"/>
+    </row>
+    <row r="34" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O34" s="23"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>43</v>
       </c>
@@ -1640,8 +1680,9 @@
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
       <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O35" s="21"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B36" s="35" t="s">
         <v>57</v>
       </c>
@@ -1657,8 +1698,9 @@
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="5"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O36" s="21"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B37" s="36" t="s">
         <v>52</v>
       </c>
@@ -1674,8 +1716,9 @@
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="5"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O37" s="21"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B38" s="36" t="s">
         <v>76</v>
       </c>
@@ -1691,8 +1734,9 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="5"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O38" s="21"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B39" s="36" t="s">
         <v>53</v>
       </c>
@@ -1708,8 +1752,9 @@
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="5"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O39" s="21"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B40" s="36" t="s">
         <v>54</v>
       </c>
@@ -1725,8 +1770,9 @@
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
       <c r="N40" s="5"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O40" s="21"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B41" s="36" t="s">
         <v>79</v>
       </c>
@@ -1742,8 +1788,9 @@
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="5"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O41" s="21"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B42" s="36" t="s">
         <v>81</v>
       </c>
@@ -1759,8 +1806,9 @@
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="5"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B43" s="36"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -1774,8 +1822,9 @@
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
       <c r="N43" s="5"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O43" s="21"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B44" s="44" t="s">
         <v>58</v>
       </c>
@@ -1791,8 +1840,9 @@
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="5"/>
-    </row>
-    <row r="45" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="O44" s="21"/>
+    </row>
+    <row r="45" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="B45" s="4" t="s">
         <v>59</v>
       </c>
@@ -1812,8 +1862,9 @@
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="5"/>
-    </row>
-    <row r="46" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="O45" s="21"/>
+    </row>
+    <row r="46" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
         <v>60</v>
       </c>
@@ -1834,8 +1885,9 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="5"/>
-    </row>
-    <row r="47" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O46" s="21"/>
+    </row>
+    <row r="47" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
         <v>67</v>
       </c>
@@ -1855,8 +1907,9 @@
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
       <c r="N47" s="5"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O47" s="21"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B48" s="4" t="s">
         <v>56</v>
       </c>
@@ -1876,8 +1929,9 @@
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
       <c r="N48" s="5"/>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="O48" s="21"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
         <v>3</v>
       </c>
@@ -1897,8 +1951,9 @@
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
       <c r="N49" s="5"/>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="O49" s="21"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B50" s="43" t="s">
         <v>4</v>
       </c>
@@ -1919,8 +1974,9 @@
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="5"/>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="O50" s="21"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B51" s="36"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -1934,8 +1990,9 @@
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
       <c r="N51" s="5"/>
-    </row>
-    <row r="52" spans="2:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="O51" s="21"/>
+    </row>
+    <row r="52" spans="2:15" ht="58" x14ac:dyDescent="0.35">
       <c r="B52" s="45" t="s">
         <v>11</v>
       </c>
@@ -1969,8 +2026,9 @@
       <c r="N52" s="49" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="O52" s="52"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B53" s="36" t="s">
         <v>63</v>
       </c>
@@ -2013,8 +2071,9 @@
         <f>ROUND(M53,2)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="54" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O53" s="21"/>
+    </row>
+    <row r="54" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B54" s="11" t="s">
         <v>64</v>
       </c>
@@ -2057,17 +2116,18 @@
         <f>ROUND(M54,2)</f>
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="O54" s="21"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C55" s="10"/>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>72</v>
       </c>
       <c r="C56" s="10"/>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B57" s="37" t="s">
         <v>62</v>
       </c>
@@ -2080,12 +2140,12 @@
       <c r="I57" s="21"/>
       <c r="J57" s="21"/>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>78</v>
       </c>

</xml_diff>